<commit_message>
Loop Unrolling Factor 2 vivado reports aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/LoopUnrollingFactor2Solution/power/LoopUnrollingFactor2BRAMPowerReport.xlsx
+++ b/reports/vivado/LoopUnrollingFactor2Solution/power/LoopUnrollingFactor2BRAMPowerReport.xlsx
@@ -80,7 +80,7 @@
     <t>RAMB36</t>
   </si>
   <si>
-    <t>ap_clk_IBUF</t>
+    <t>ap_clk_IBUF_BUFG</t>
   </si>
   <si>
     <t>WRITE_FIRST</t>
@@ -245,7 +245,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>0.0021069447975605726</v>
+        <v>0.0012505515478551388</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>18</v>
@@ -301,7 +301,7 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>0.0021069447975605726</v>
+        <v>0.0012505515478551388</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>20</v>
@@ -310,7 +310,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>16.388080596923828</v>
+        <v>9.324859619140625</v>
       </c>
       <c r="E3" t="s" s="4">
         <v>22</v>
@@ -319,7 +319,7 @@
         <v>100.0</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>48.56139373779297</v>
+        <v>19.671045303344727</v>
       </c>
       <c r="H3" t="n" s="7">
         <v>36.0</v>
@@ -331,7 +331,7 @@
         <v>23</v>
       </c>
       <c r="K3" t="n" s="2">
-        <v>16.744186401367188</v>
+        <v>10.667463302612305</v>
       </c>
       <c r="L3" t="s" s="4">
         <v>22</v>
@@ -340,7 +340,7 @@
         <v>100.0</v>
       </c>
       <c r="N3" t="n" s="2">
-        <v>48.56139373779297</v>
+        <v>39.26985168457031</v>
       </c>
       <c r="O3" t="n" s="7">
         <v>36.0</v>
@@ -352,7 +352,7 @@
         <v>23</v>
       </c>
       <c r="R3" t="n" s="2">
-        <v>16.744186401367188</v>
+        <v>8.95522403717041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>